<commit_message>
Works with multiple files in folder
</commit_message>
<xml_diff>
--- a/total.xlsx
+++ b/total.xlsx
@@ -1,25 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\python_lps_attendance\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Total" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="26">
   <si>
     <t>Student Number</t>
   </si>
@@ -36,10 +31,13 @@
     <t>Form</t>
   </si>
   <si>
+    <t>Cersie</t>
+  </si>
+  <si>
     <t>Ned</t>
   </si>
   <si>
-    <t>Cersie</t>
+    <t>Margery</t>
   </si>
   <si>
     <t>Rickon</t>
@@ -51,22 +49,22 @@
     <t>Samwell</t>
   </si>
   <si>
-    <t>Margery</t>
-  </si>
-  <si>
     <t>Arya</t>
   </si>
   <si>
+    <t>Danaerys</t>
+  </si>
+  <si>
     <t>Jamie</t>
   </si>
   <si>
-    <t>Danaerys</t>
+    <t>Lannister</t>
   </si>
   <si>
     <t>Stark</t>
   </si>
   <si>
-    <t>Lannister</t>
+    <t>Tyrell</t>
   </si>
   <si>
     <t>Snow</t>
@@ -75,25 +73,22 @@
     <t>Tarley</t>
   </si>
   <si>
-    <t>Tyrell</t>
-  </si>
-  <si>
     <t>Targaryan</t>
   </si>
   <si>
+    <t>3B</t>
+  </si>
+  <si>
     <t>1A</t>
   </si>
   <si>
-    <t>3B</t>
+    <t>4A</t>
   </si>
   <si>
     <t>3A</t>
   </si>
   <si>
     <t>2C</t>
-  </si>
-  <si>
-    <t>4A</t>
   </si>
   <si>
     <t>6A</t>
@@ -102,8 +97,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,14 +161,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -220,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -252,10 +239,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -287,7 +273,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -463,23 +448,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="15.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.5703125" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -496,12 +472,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2">
-        <v>1240</v>
+        <v>1236</v>
       </c>
       <c r="B2">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -513,12 +489,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3">
-        <v>1236</v>
+        <v>1240</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
@@ -530,80 +506,80 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4">
-        <v>1585</v>
+        <v>1242</v>
       </c>
       <c r="B4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5">
-        <v>1234</v>
+        <v>1585</v>
       </c>
       <c r="B5">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
         <v>8</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6">
-        <v>1238</v>
+        <v>1241</v>
       </c>
       <c r="B6">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>9</v>
-      </c>
       <c r="D6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7">
-        <v>2145</v>
+        <v>1234</v>
       </c>
       <c r="B7">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8">
+        <v>1238</v>
+      </c>
+      <c r="B8">
         <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>1654</v>
-      </c>
-      <c r="B8">
-        <v>6</v>
       </c>
       <c r="C8" t="s">
         <v>10</v>
@@ -615,139 +591,241 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9">
-        <v>1239</v>
+        <v>9999</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s">
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E9" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10">
-        <v>1542</v>
+        <v>8888</v>
       </c>
       <c r="B10">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D10" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11">
-        <v>1235</v>
+        <v>5454</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
       </c>
       <c r="D11" t="s">
+        <v>19</v>
+      </c>
+      <c r="E11" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12">
+        <v>6565</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13">
+        <v>4545</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14">
+        <v>1111</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" t="s">
         <v>15</v>
       </c>
-      <c r="E11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>1354</v>
-      </c>
-      <c r="B12">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>12</v>
-      </c>
-      <c r="D12" t="s">
-        <v>15</v>
-      </c>
-      <c r="E12" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>1242</v>
-      </c>
-      <c r="B13">
-        <v>3</v>
-      </c>
-      <c r="C13" t="s">
-        <v>10</v>
-      </c>
-      <c r="D13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>1237</v>
-      </c>
-      <c r="B14">
-        <v>2</v>
-      </c>
-      <c r="C14" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
-      </c>
       <c r="E14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15">
-        <v>1241</v>
+        <v>1654</v>
       </c>
       <c r="B15">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C15" t="s">
         <v>7</v>
       </c>
       <c r="D15" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5">
       <c r="A16">
+        <v>2145</v>
+      </c>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
+        <v>17</v>
+      </c>
+      <c r="E16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17">
+        <v>1542</v>
+      </c>
+      <c r="B17">
+        <v>5</v>
+      </c>
+      <c r="C17" t="s">
+        <v>11</v>
+      </c>
+      <c r="D17" t="s">
+        <v>15</v>
+      </c>
+      <c r="E17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18">
+        <v>1239</v>
+      </c>
+      <c r="B18">
+        <v>5</v>
+      </c>
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>15</v>
+      </c>
+      <c r="E18" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19">
+        <v>1235</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20">
+        <v>1354</v>
+      </c>
+      <c r="B20">
+        <v>4</v>
+      </c>
+      <c r="C20" t="s">
+        <v>13</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21">
         <v>1988</v>
       </c>
-      <c r="B16">
+      <c r="B21">
         <v>2</v>
       </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
+      <c r="C21" t="s">
+        <v>12</v>
+      </c>
+      <c r="D21" t="s">
         <v>19</v>
       </c>
-      <c r="E16" t="s">
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22">
+        <v>1237</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" t="s">
+        <v>19</v>
+      </c>
+      <c r="E22" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Functionality to add reasons dynamically
</commit_message>
<xml_diff>
--- a/total.xlsx
+++ b/total.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="40">
   <si>
     <t>Student Number</t>
   </si>
@@ -34,6 +34,24 @@
     <t>Total Attendance %</t>
   </si>
   <si>
+    <t>W1</t>
+  </si>
+  <si>
+    <t>W1 Reason</t>
+  </si>
+  <si>
+    <t>W2</t>
+  </si>
+  <si>
+    <t>W2 Reason</t>
+  </si>
+  <si>
+    <t>W3</t>
+  </si>
+  <si>
+    <t>W3 Reason</t>
+  </si>
+  <si>
     <t>Cersie</t>
   </si>
   <si>
@@ -95,6 +113,27 @@
   </si>
   <si>
     <t>6A</t>
+  </si>
+  <si>
+    <t>Dentist</t>
+  </si>
+  <si>
+    <t>Ill</t>
+  </si>
+  <si>
+    <t>Doctors</t>
+  </si>
+  <si>
+    <t>Trip</t>
+  </si>
+  <si>
+    <t>Not Well</t>
+  </si>
+  <si>
+    <t>Holiday</t>
+  </si>
+  <si>
+    <t>Unauthorised</t>
   </si>
 </sst>
 </file>
@@ -452,13 +491,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -477,19 +516,37 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1236</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>20</v>
@@ -497,19 +554,37 @@
       <c r="F2">
         <v>58.75</v>
       </c>
-    </row>
-    <row r="3" spans="1:6">
+      <c r="G2">
+        <v>5</v>
+      </c>
+      <c r="H2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>1240</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>16</v>
@@ -517,19 +592,31 @@
       <c r="F3">
         <v>65</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
+      <c r="G3">
+        <v>9</v>
+      </c>
+      <c r="H3" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3">
+        <v>7</v>
+      </c>
+      <c r="J3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>1242</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E4">
         <v>10</v>
@@ -537,19 +624,31 @@
       <c r="F4">
         <v>67.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:6">
+      <c r="G4">
+        <v>3</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K4">
+        <v>7</v>
+      </c>
+      <c r="L4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>1585</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E5">
         <v>9</v>
@@ -557,19 +656,25 @@
       <c r="F5">
         <v>85</v>
       </c>
-    </row>
-    <row r="6" spans="1:6">
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>1241</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="E6">
         <v>9</v>
@@ -577,19 +682,31 @@
       <c r="F6">
         <v>75</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
+      <c r="K6">
+        <v>7</v>
+      </c>
+      <c r="L6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>1234</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E7">
         <v>8</v>
@@ -597,19 +714,25 @@
       <c r="F7">
         <v>75</v>
       </c>
-    </row>
-    <row r="8" spans="1:6">
+      <c r="G7">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>1238</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E8">
         <v>8</v>
@@ -617,19 +740,31 @@
       <c r="F8">
         <v>62.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:6">
+      <c r="G8">
+        <v>7</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9">
         <v>9999</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E9">
         <v>7</v>
@@ -637,19 +772,25 @@
       <c r="F9">
         <v>100</v>
       </c>
-    </row>
-    <row r="10" spans="1:6">
+      <c r="K9">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10">
         <v>8888</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="D10" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E10">
         <v>7</v>
@@ -657,19 +798,25 @@
       <c r="F10">
         <v>100</v>
       </c>
-    </row>
-    <row r="11" spans="1:6">
+      <c r="K10">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>5454</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D11" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E11">
         <v>7</v>
@@ -677,19 +824,25 @@
       <c r="F11">
         <v>50</v>
       </c>
-    </row>
-    <row r="12" spans="1:6">
+      <c r="K11">
+        <v>7</v>
+      </c>
+      <c r="L11" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>6565</v>
       </c>
       <c r="B12" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E12">
         <v>7</v>
@@ -697,19 +850,25 @@
       <c r="F12">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="1:6">
+      <c r="K12">
+        <v>7</v>
+      </c>
+      <c r="L12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>4545</v>
       </c>
       <c r="B13" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C13" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E13">
         <v>7</v>
@@ -717,19 +876,25 @@
       <c r="F13">
         <v>35</v>
       </c>
-    </row>
-    <row r="14" spans="1:6">
+      <c r="K13">
+        <v>7</v>
+      </c>
+      <c r="L13" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>1111</v>
       </c>
       <c r="B14" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E14">
         <v>7</v>
@@ -737,19 +902,25 @@
       <c r="F14">
         <v>100</v>
       </c>
-    </row>
-    <row r="15" spans="1:6">
+      <c r="K14">
+        <v>7</v>
+      </c>
+      <c r="L14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>1654</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="D15" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="E15">
         <v>6</v>
@@ -757,19 +928,25 @@
       <c r="F15">
         <v>85</v>
       </c>
-    </row>
-    <row r="16" spans="1:6">
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>2145</v>
       </c>
       <c r="B16" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E16">
         <v>6</v>
@@ -777,19 +954,25 @@
       <c r="F16">
         <v>45</v>
       </c>
-    </row>
-    <row r="17" spans="1:6">
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10">
       <c r="A17">
         <v>1542</v>
       </c>
       <c r="B17" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C17" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E17">
         <v>5</v>
@@ -797,19 +980,25 @@
       <c r="F17">
         <v>75</v>
       </c>
-    </row>
-    <row r="18" spans="1:6">
+      <c r="I17">
+        <v>5</v>
+      </c>
+      <c r="J17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10">
       <c r="A18">
         <v>1239</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="E18">
         <v>5</v>
@@ -817,19 +1006,25 @@
       <c r="F18">
         <v>35</v>
       </c>
-    </row>
-    <row r="19" spans="1:6">
+      <c r="G18">
+        <v>5</v>
+      </c>
+      <c r="H18" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10">
       <c r="A19">
         <v>1235</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D19" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E19">
         <v>4</v>
@@ -837,19 +1032,25 @@
       <c r="F19">
         <v>66</v>
       </c>
-    </row>
-    <row r="20" spans="1:6">
+      <c r="G19">
+        <v>4</v>
+      </c>
+      <c r="H19" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10">
       <c r="A20">
         <v>1354</v>
       </c>
       <c r="B20" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C20" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D20" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E20">
         <v>4</v>
@@ -857,19 +1058,25 @@
       <c r="F20">
         <v>45</v>
       </c>
-    </row>
-    <row r="21" spans="1:6">
+      <c r="I20">
+        <v>4</v>
+      </c>
+      <c r="J20" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21">
         <v>1988</v>
       </c>
       <c r="B21" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D21" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E21">
         <v>2</v>
@@ -877,25 +1084,37 @@
       <c r="F21">
         <v>50</v>
       </c>
-    </row>
-    <row r="22" spans="1:6">
+      <c r="I21">
+        <v>2</v>
+      </c>
+      <c r="J21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
       <c r="A22">
         <v>1237</v>
       </c>
       <c r="B22" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C22" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="D22" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="E22">
         <v>2</v>
       </c>
       <c r="F22">
         <v>100</v>
+      </c>
+      <c r="G22">
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>